<commit_message>
Actualización de proyectos - Proy 03 y 04
</commit_message>
<xml_diff>
--- a/Power Bi/Resumen de proyectos.xlsx
+++ b/Power Bi/Resumen de proyectos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Portfolio - GD\Portfolio - Power BI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Portfolio - GD\Portfolio\Power Bi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3983A5D5-4B37-4920-AFAB-B13CE68259AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A934ED-A073-4723-8639-082AEC7FC527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2AABFEF9-04FB-471C-8AE7-B19FAD1FE54B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>INTRODUCCION</t>
   </si>
@@ -107,12 +107,55 @@
       <t>me muestre como estoy en un período y compararlo con otro.</t>
     </r>
   </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiMDM0MTQ3YTEtOWQ3Ni00ODk5LWFjMDgtYjYwYWU3YzE4NTQ5IiwidCI6IjkxZjVjYjg5LTUyZmUtNDdhYi05MDVmLTRlMzU4ODZmNWE1NyIsImMiOjR9</t>
+  </si>
+  <si>
+    <t>Proy_03 - Seguimiento de stocks</t>
+  </si>
+  <si>
+    <r>
+      <t>Desarrollé este tablero con el objeto de controlar y analizar los stocks de materia prima y productos elaborados. Además le adhiero un grafico de ciclos para el analisis de la estacionalidades a lo largo de los años</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Datos estimados. Se editaron los datos reales pero se generaron sintéticos que mantuvieran una tendencia parecida.</t>
+  </si>
+  <si>
+    <t>Con python. En la carpeta dataset se encuentra el notebook.</t>
+  </si>
+  <si>
+    <t>https://app.powerbi.com/view?r=eyJrIjoiNjkxMTZmOGEtMzJhNi00OGRlLTg3OGEtMGU1YzJmNDc0OTE1IiwidCI6IjkxZjVjYjg5LTUyZmUtNDdhYi05MDVmLTRlMzU4ODZmNWE1NyIsImMiOjR9</t>
+  </si>
+  <si>
+    <t>Proy_04 - Data - Proyecto final</t>
+  </si>
+  <si>
+    <t>Presenté este tablero como proyecto final para la diplomatura en Ciencia de Datos. El tablero presenta redundancias pero se ajustó a los requisitos del proyceto que solicitó Coderhouser</t>
+  </si>
+  <si>
+    <t>Dataset dado por Coderhouse</t>
+  </si>
+  <si>
+    <t>Powerquery</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +175,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,7 +209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -173,6 +224,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -490,19 +544,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80916508-CA75-4B85-BBD8-0BDF3F970ECE}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1048576"/>
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="88" style="1" customWidth="1"/>
+    <col min="2" max="4" width="88" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="88" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -512,8 +567,14 @@
       <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="270" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="270" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -523,8 +584,14 @@
       <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -534,8 +601,14 @@
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -545,8 +618,14 @@
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -556,8 +635,14 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -566,6 +651,12 @@
       </c>
       <c r="C6" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>